<commit_message>
still trying to commit
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/similarity_scores_courses.xlsx
+++ b/AIacademia/data_files/similarity_scores_courses.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2366857629772701</v>
+        <v>0.2225729989246953</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1364974908840263</v>
+        <v>0.2185938719739137</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1767696348166654</v>
+        <v>0.1580244899580968</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1594694472454184</v>
+        <v>0.1993691068915476</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1761179050029809</v>
+        <v>0.1919427087949038</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2065413278435502</v>
+        <v>0.2199786617192732</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1635777162744473</v>
+        <v>0.1762347010727719</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1776328739719876</v>
+        <v>0.1547639014287874</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3020502538863964</v>
+        <v>0.2515899659146517</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2229706408037189</v>
+        <v>0.2115133208638662</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1196725691833904</v>
+        <v>0.07994217227245783</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1957567598406083</v>
+        <v>0.172461673725689</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.136789526100054</v>
+        <v>0.1703472908511281</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1551587971324636</v>
+        <v>0.2065557988038792</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1953485826887082</v>
+        <v>0.1871266035253376</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2337452729294386</v>
+        <v>0.264368031372667</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1633166454097791</v>
+        <v>0.2034974490027841</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.2383166639222602</v>
+        <v>0.1916350931379784</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1919761188336963</v>
+        <v>0.1780546825999253</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.162924786820819</v>
+        <v>0.196022225772513</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1689562299702253</v>
+        <v>0.1214537175050256</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.2018777038085708</v>
+        <v>0.1533154264735849</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1003091815805886</v>
+        <v>0.1332916530968697</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1707087113720783</v>
+        <v>0.2028324594284665</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.206436706453036</v>
+        <v>0.1875431948010683</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.2810319426275454</v>
+        <v>0.2577515256473847</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.2877659964967076</v>
+        <v>0.3090118166696694</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.1195775048482588</v>
+        <v>0.09961865905658623</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.2124586645577557</v>
+        <v>0.1811816623748037</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.2071033712097314</v>
+        <v>0.2826938213572558</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.158039565034169</v>
+        <v>0.1647730418862527</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1534962037767999</v>
+        <v>0.1209942430837056</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1779064112976012</v>
+        <v>0.1900194850035571</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.1903439746755231</v>
+        <v>0.1703648828900786</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.213808479009231</v>
+        <v>0.1281530041310535</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.2233563018624382</v>
+        <v>0.2341392414443393</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.199742785575289</v>
+        <v>0.2196548221740449</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.2084018683633853</v>
+        <v>0.1834853024030706</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.215892720930329</v>
+        <v>0.2387031307088887</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1942143017280813</v>
+        <v>0.1613517033335533</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.2122778674589597</v>
+        <v>0.1763442277687054</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.1871043139329264</v>
+        <v>0.2828034277999462</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.2303339319518015</v>
+        <v>0.2309564765118704</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2601670871536301</v>
+        <v>0.3246354056666368</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.1494448285568172</v>
+        <v>0.1225666453223031</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.2184100452251666</v>
+        <v>0.3235611708349139</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.2350486176784622</v>
+        <v>0.1668956897754365</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.2190292750780387</v>
+        <v>0.1851920853771044</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.2480659032149212</v>
+        <v>0.1619949994789993</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.2718518084164135</v>
+        <v>0.1813831568987349</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2177556778441796</v>
+        <v>0.2042228323230325</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.1449803293943611</v>
+        <v>0.2098196311646337</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.2160485370045748</v>
+        <v>0.1949395146105441</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.2534016871425371</v>
+        <v>0.2430204226917999</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.1687988129891115</v>
+        <v>0.1263052408444525</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.1509533515673689</v>
+        <v>0.1121952593176505</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.2291417060221068</v>
+        <v>0.1911460885545064</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.2151328906766993</v>
+        <v>0.2065230419227556</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.2887927691374919</v>
+        <v>0.330770000388631</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.2515148282576174</v>
+        <v>0.2041524140415935</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.1036650392660823</v>
+        <v>0.08326611516521817</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.1486820541717002</v>
+        <v>0.1643457523645145</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.2315858140136471</v>
+        <v>0.1968364552068901</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.1116861056316403</v>
+        <v>0.1139138937921707</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1295331325902229</v>
+        <v>0.1482483440962012</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1971084461898227</v>
+        <v>0.1736791764473961</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.2008484146431784</v>
+        <v>0.2591984599955779</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.1575726135318729</v>
+        <v>0.1717094003668587</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.2231474967763287</v>
+        <v>0.2117724920535764</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.2186843574276625</v>
+        <v>0.1883695874210866</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.2465152688707824</v>
+        <v>0.2566390044911464</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.2299845813146053</v>
+        <v>0.2219694921722728</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.2223183501303269</v>
+        <v>0.1456063870285668</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.1031009757506968</v>
+        <v>0.1631545997309555</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.1475873686526041</v>
+        <v>0.1174998185196909</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.1558463957516396</v>
+        <v>0.1484457714358207</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.189250962553312</v>
+        <v>0.155349601895375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comparing two styles of finding recommendations, word vs sentence clustering, while trying with different numbers of kmeans clusters
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/similarity_scores_courses.xlsx
+++ b/AIacademia/data_files/similarity_scores_courses.xlsx
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1580244899580968</v>
+        <v>0.1614932821685667</v>
       </c>
     </row>
     <row r="5">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1919427087949038</v>
+        <v>0.2023608905510596</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2199786617192732</v>
+        <v>0.2211020455267163</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1762347010727719</v>
+        <v>0.1766371156411559</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1547639014287874</v>
+        <v>0.1414627756152198</v>
       </c>
     </row>
     <row r="10">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2115133208638662</v>
+        <v>0.226444284693467</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.07994217227245783</v>
+        <v>0.08769308169122851</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.172461673725689</v>
+        <v>0.1435805489676914</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1703472908511281</v>
+        <v>0.1624484649590589</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.2065557988038792</v>
+        <v>0.1731355958147772</v>
       </c>
     </row>
     <row r="16">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.264368031372667</v>
+        <v>0.1916233172933781</v>
       </c>
     </row>
     <row r="18">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.1916350931379784</v>
+        <v>0.2287516070550251</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1780546825999253</v>
+        <v>0.1736546478030555</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.196022225772513</v>
+        <v>0.1848761074453971</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1214537175050256</v>
+        <v>0.1713699259368486</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.1533154264735849</v>
+        <v>0.1779696044714125</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1332916530968697</v>
+        <v>0.1404030286485607</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.2028324594284665</v>
+        <v>0.2022389753616026</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1875431948010683</v>
+        <v>0.1912384331656097</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.2577515256473847</v>
+        <v>0.2541806191132886</v>
       </c>
     </row>
     <row r="28">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.09961865905658623</v>
+        <v>0.1019587035736605</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.1811816623748037</v>
+        <v>0.2365928227144809</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.2826938213572558</v>
+        <v>0.2846227786979708</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.1647730418862527</v>
+        <v>0.1766573030530097</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1209942430837056</v>
+        <v>0.133329554673875</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1900194850035571</v>
+        <v>0.1900616305511722</v>
       </c>
     </row>
     <row r="35">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.1281530041310535</v>
+        <v>0.1437153912033442</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.2341392414443393</v>
+        <v>0.2056578078520161</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.2196548221740449</v>
+        <v>0.2345243472556311</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.1834853024030706</v>
+        <v>0.1610943787723742</v>
       </c>
     </row>
     <row r="40">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1613517033335533</v>
+        <v>0.1458240755039918</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.1763442277687054</v>
+        <v>0.2059327919499025</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.2828034277999462</v>
+        <v>0.2838018152548218</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.2309564765118704</v>
+        <v>0.1931262228905267</v>
       </c>
     </row>
     <row r="45">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.1225666453223031</v>
+        <v>0.1199325929446099</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.3235611708349139</v>
+        <v>0.3067553465909482</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.1668956897754365</v>
+        <v>0.1570109909858135</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.1851920853771044</v>
+        <v>0.1468919994367651</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.1619949994789993</v>
+        <v>0.1691606932123232</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.1813831568987349</v>
+        <v>0.1741003377770491</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2042228323230325</v>
+        <v>0.1707944155372615</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.2098196311646337</v>
+        <v>0.1731564074651663</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.1949395146105441</v>
+        <v>0.2066678131385672</v>
       </c>
     </row>
     <row r="55">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.1263052408444525</v>
+        <v>0.1307145141641815</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.1121952593176505</v>
+        <v>0.1079885373714472</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.1911460885545064</v>
+        <v>0.19053454548198</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.2065230419227556</v>
+        <v>0.1919971538337066</v>
       </c>
     </row>
     <row r="60">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.2041524140415935</v>
+        <v>0.2523508369705812</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.08326611516521817</v>
+        <v>0.08738840731918887</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.1643457523645145</v>
+        <v>0.1317842032747991</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.1968364552068901</v>
+        <v>0.2194312291951577</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.1139138937921707</v>
+        <v>0.1060408619463494</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1482483440962012</v>
+        <v>0.1351086119716099</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1736791764473961</v>
+        <v>0.1730950473408821</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.2591984599955779</v>
+        <v>0.2893374763815736</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.1717094003668587</v>
+        <v>0.1856236362155468</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.2117724920535764</v>
+        <v>0.2173390525439929</v>
       </c>
     </row>
     <row r="71">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.2566390044911464</v>
+        <v>0.2793372305797195</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.2219694921722728</v>
+        <v>0.2442622511631537</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.1456063870285668</v>
+        <v>0.1492557098424128</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.1631545997309555</v>
+        <v>0.138045466837423</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.1174998185196909</v>
+        <v>0.1305344264377558</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.1484457714358207</v>
+        <v>0.1447337515325399</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.155349601895375</v>
+        <v>0.1493412722513493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
proacted 1.2 sentence tokenization, dumping word tokenization model
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/similarity_scores_courses.xlsx
+++ b/AIacademia/data_files/similarity_scores_courses.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2225729989246953</v>
+        <v>0.2377347397804473</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2185938719739137</v>
+        <v>0.1543604700559567</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1614932821685667</v>
+        <v>0.251585782613469</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1993691068915476</v>
+        <v>0.1494280070122514</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2023608905510596</v>
+        <v>0.1354613017779132</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2211020455267163</v>
+        <v>0.2650730800634213</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1766371156411559</v>
+        <v>0.2344869295150573</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1414627756152198</v>
+        <v>0.1464603184485922</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2515899659146517</v>
+        <v>0.2113211214126457</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.226444284693467</v>
+        <v>0.2075638418632239</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.08769308169122851</v>
+        <v>0.1665166353100112</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1435805489676914</v>
+        <v>0.1579540858194672</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1624484649590589</v>
+        <v>0.1652945669008024</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1731355958147772</v>
+        <v>0.1645562403779922</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1871266035253376</v>
+        <v>0.182182048665788</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1916233172933781</v>
+        <v>0.2219619050606416</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.2034974490027841</v>
+        <v>0.09117381186172682</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.2287516070550251</v>
+        <v>0.2632210332655361</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1736546478030555</v>
+        <v>0.1820906027470262</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.1848761074453971</v>
+        <v>0.1571869149263968</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1713699259368486</v>
+        <v>0.1666665446218413</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.1779696044714125</v>
+        <v>0.1889785612249422</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1404030286485607</v>
+        <v>0.08767079386919532</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.2022389753616026</v>
+        <v>0.1721018354523523</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1912384331656097</v>
+        <v>0.2742781765229103</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.2541806191132886</v>
+        <v>0.1951429116059076</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.3090118166696694</v>
+        <v>0.3070528500481298</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.1019587035736605</v>
+        <v>0.1439333127970953</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.2365928227144809</v>
+        <v>0.192540509710008</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.2846227786979708</v>
+        <v>0.3022253590717894</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.1766573030530097</v>
+        <v>0.1705504073475237</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.133329554673875</v>
+        <v>0.1842622732743352</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1900616305511722</v>
+        <v>0.2013297374803324</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.1703648828900786</v>
+        <v>0.1924914849925276</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.1437153912033442</v>
+        <v>0.1764049565438014</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.2056578078520161</v>
+        <v>0.205713429138442</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.2345243472556311</v>
+        <v>0.241736018927826</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.1610943787723742</v>
+        <v>0.1511705503875471</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.2387031307088887</v>
+        <v>0.2092311324332255</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1458240755039918</v>
+        <v>0.2027128115013695</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.2059327919499025</v>
+        <v>0.1940841778297292</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.2838018152548218</v>
+        <v>0.1546303521256976</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.1931262228905267</v>
+        <v>0.1573236815058442</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.3246354056666368</v>
+        <v>0.2093296792365324</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.1199325929446099</v>
+        <v>0.1641695163468298</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.3067553465909482</v>
+        <v>0.2452345544152963</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.1570109909858135</v>
+        <v>0.214120442639659</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.1468919994367651</v>
+        <v>0.2019740948408203</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.1691606932123232</v>
+        <v>0.2275177740135915</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.1741003377770491</v>
+        <v>0.1688688910828539</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.1707944155372615</v>
+        <v>0.2583928921774317</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.1731564074651663</v>
+        <v>0.1714816158709366</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.2066678131385672</v>
+        <v>0.1876586990065328</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.2430204226917999</v>
+        <v>0.2688365548518937</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.1307145141641815</v>
+        <v>0.2286832407029697</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.1079885373714472</v>
+        <v>0.118770108077467</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.19053454548198</v>
+        <v>0.2510735196905842</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.1919971538337066</v>
+        <v>0.2313059547443149</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.330770000388631</v>
+        <v>0.224577544702168</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.2523508369705812</v>
+        <v>0.2323060716593902</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.08738840731918887</v>
+        <v>0.16973509223877</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.1317842032747991</v>
+        <v>0.152090954373878</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.2194312291951577</v>
+        <v>0.2400130043555971</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.1060408619463494</v>
+        <v>0.1920021496176086</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1351086119716099</v>
+        <v>0.1881974001442445</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1730950473408821</v>
+        <v>0.218009627802776</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.2893374763815736</v>
+        <v>0.1713604323410646</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.1856236362155468</v>
+        <v>0.1934907850019723</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.2173390525439929</v>
+        <v>0.1688317038968409</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.1883695874210866</v>
+        <v>0.1697854750245221</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.2793372305797195</v>
+        <v>0.2095644747452401</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.2442622511631537</v>
+        <v>0.1944915149864047</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.1492557098424128</v>
+        <v>0.16980769471393</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.138045466837423</v>
+        <v>0.2023392561536684</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.1305344264377558</v>
+        <v>0.1830764900074947</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.1447337515325399</v>
+        <v>0.1653809993627637</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.1493412722513493</v>
+        <v>0.1633942294992086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
objectives now ready to be clustered to form 3000 dimmensional sets
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/similarity_scores_courses.xlsx
+++ b/AIacademia/data_files/similarity_scores_courses.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2377347397804473</v>
+        <v>0.3031030526911432</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1543604700559567</v>
+        <v>0.2646759527437429</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.251585782613469</v>
+        <v>0.3010672122217473</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1494280070122514</v>
+        <v>0.1857996930693342</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1354613017779132</v>
+        <v>0.2666843482755799</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2650730800634213</v>
+        <v>0.3172781833158986</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2344869295150573</v>
+        <v>0.2299262201533056</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1464603184485922</v>
+        <v>0.1585231062812161</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2113211214126457</v>
+        <v>0.2528836928636566</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2075638418632239</v>
+        <v>0.2452752211742054</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1665166353100112</v>
+        <v>0.2330846907205628</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1579540858194672</v>
+        <v>0.1541328817397854</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1652945669008024</v>
+        <v>0.1553962895637222</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1645562403779922</v>
+        <v>0.200170376090257</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.182182048665788</v>
+        <v>0.1925777228317418</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2219619050606416</v>
+        <v>0.2769683683347696</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.09117381186172682</v>
+        <v>0.1882054782319281</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.2632210332655361</v>
+        <v>0.2721188087233145</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1820906027470262</v>
+        <v>0.1911858187425866</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.1571869149263968</v>
+        <v>0.1405487327526666</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1666665446218413</v>
+        <v>0.1729847822153952</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.1889785612249422</v>
+        <v>0.2356496246225906</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.08767079386919532</v>
+        <v>0.09340496781451638</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1721018354523523</v>
+        <v>0.1505483795509852</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.2742781765229103</v>
+        <v>0.3400593326103616</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.1951429116059076</v>
+        <v>0.254978200374293</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.3070528500481298</v>
+        <v>0.3759860926245485</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.1439333127970953</v>
+        <v>0.1525970846734771</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.192540509710008</v>
+        <v>0.1743923826218427</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3022253590717894</v>
+        <v>0.3441678189982821</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.1705504073475237</v>
+        <v>0.2325964039055812</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1842622732743352</v>
+        <v>0.2121344956696883</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.2013297374803324</v>
+        <v>0.1657202540739919</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.1924914849925276</v>
+        <v>0.2715570107686192</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.1764049565438014</v>
+        <v>0.2331038502111906</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.205713429138442</v>
+        <v>0.2015050752556725</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.241736018927826</v>
+        <v>0.2192844718281782</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.1511705503875471</v>
+        <v>0.2069714739096859</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.2092311324332255</v>
+        <v>0.3383885801018612</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.2027128115013695</v>
+        <v>0.2098195939482268</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.1940841778297292</v>
+        <v>0.2137179949074502</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.1546303521256976</v>
+        <v>0.1795789737747447</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.1573236815058442</v>
+        <v>0.1646274532176297</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2093296792365324</v>
+        <v>0.2829194960814491</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.1641695163468298</v>
+        <v>0.2141019023010011</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.2452345544152963</v>
+        <v>0.3022534919263937</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.214120442639659</v>
+        <v>0.2231995161195222</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.2019740948408203</v>
+        <v>0.2879264174706963</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.2275177740135915</v>
+        <v>0.3292303017393478</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.1688688910828539</v>
+        <v>0.3048772031524299</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2583928921774317</v>
+        <v>0.3199931504041301</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.1714816158709366</v>
+        <v>0.2201985347700067</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.1876586990065328</v>
+        <v>0.190220833396446</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.2688365548518937</v>
+        <v>0.3809247416287085</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.2286832407029697</v>
+        <v>0.3070507106522474</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.118770108077467</v>
+        <v>0.2051082819470727</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.2510735196905842</v>
+        <v>0.2236368798603683</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.2313059547443149</v>
+        <v>0.2582662286735862</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.224577544702168</v>
+        <v>0.2627729081303424</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.2323060716593902</v>
+        <v>0.2515903309412535</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.16973509223877</v>
+        <v>0.2279808317248863</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.152090954373878</v>
+        <v>0.1880846368812956</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.2400130043555971</v>
+        <v>0.3088656210444864</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.1920021496176086</v>
+        <v>0.4026998536267705</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1881974001442445</v>
+        <v>0.2882974624343621</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.218009627802776</v>
+        <v>0.197634552709223</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.1713604323410646</v>
+        <v>0.206237316516559</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.1934907850019723</v>
+        <v>0.2244632121384939</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.1688317038968409</v>
+        <v>0.193780622500697</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.1697854750245221</v>
+        <v>0.188221552986471</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.2095644747452401</v>
+        <v>0.294371349511847</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.1944915149864047</v>
+        <v>0.2608886591279338</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.16980769471393</v>
+        <v>0.221817571782538</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.2023392561536684</v>
+        <v>0.3541345792767692</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.1830764900074947</v>
+        <v>0.2604765439248585</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.1653809993627637</v>
+        <v>0.2371680202914283</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.1633942294992086</v>
+        <v>0.2062996703527221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Proacted Recommender system 1.3
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/similarity_scores_courses.xlsx
+++ b/AIacademia/data_files/similarity_scores_courses.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1824936751613834</v>
+        <v>0.2432490129025711</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2317473888535702</v>
+        <v>0.2411897279234069</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2376530296263142</v>
+        <v>0.2279374252521792</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1516086032871022</v>
+        <v>0.2110671728913582</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1990854234405351</v>
+        <v>0.2232835019967376</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2196813845232968</v>
+        <v>0.2338366062972175</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.203489026958722</v>
+        <v>0.2135195243514688</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1485013260084578</v>
+        <v>0.200607347540649</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1764744801046101</v>
+        <v>0.2823875815070244</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1794035352775858</v>
+        <v>0.1998897476382224</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1974074920200406</v>
+        <v>0.2053661800737224</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.2102464003209671</v>
+        <v>0.2025752555140319</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1455353771332317</v>
+        <v>0.1739384242826933</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1799508157365124</v>
+        <v>0.2015725473051372</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1859361010674234</v>
+        <v>0.2320889448780388</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1829758758944881</v>
+        <v>0.2167895105100233</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.2210789546456689</v>
+        <v>0.2144442310725814</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.191290772714984</v>
+        <v>0.2121829174672534</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1676656629257355</v>
+        <v>0.1731373828639528</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.1751824305185567</v>
+        <v>0.1940917271092404</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1738220095283137</v>
+        <v>0.2079469975294282</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.2046199182240863</v>
+        <v>0.179211919645771</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1158877922385684</v>
+        <v>0.1674113558621942</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1828970065198267</v>
+        <v>0.1897901160543019</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.2669697286264353</v>
+        <v>0.205923835628804</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.1954848763931794</v>
+        <v>0.2205501952095101</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.2136788875518469</v>
+        <v>0.2019318048492107</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.1939492007172717</v>
+        <v>0.1958749450597683</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.1847599881337664</v>
+        <v>0.1981261388742524</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.1824931771449953</v>
+        <v>0.2391133932550645</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.1885368251228011</v>
+        <v>0.1950598397699665</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1848221300218739</v>
+        <v>0.1487496675782086</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1583881705481297</v>
+        <v>0.1892665454765523</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.1762584085916622</v>
+        <v>0.1765637362566932</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.1733076713224236</v>
+        <v>0.2337421648130379</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.1548617484913297</v>
+        <v>0.196159914135432</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.1584038075523559</v>
+        <v>0.2096921815164276</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.2378545878153589</v>
+        <v>0.1988977444286743</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.2475716845020496</v>
+        <v>0.2290684984032781</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.2123844111806007</v>
+        <v>0.2153576239808776</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.2277276277178376</v>
+        <v>0.2127302161003796</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.1805944022943746</v>
+        <v>0.2123330059331108</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.1480678615449562</v>
+        <v>0.2111907239136736</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2101712129795292</v>
+        <v>0.2413968397084669</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.1793127956508198</v>
+        <v>0.1838156528288608</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.2145078450610379</v>
+        <v>0.2464650140770868</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.1860342742614958</v>
+        <v>0.2234666136291428</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.2402290535652423</v>
+        <v>0.1959046171534852</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.2365063749388666</v>
+        <v>0.2027371075584232</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.2128173532484794</v>
+        <v>0.2207704047530455</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2304778916287789</v>
+        <v>0.2514823645950497</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.1790222434576274</v>
+        <v>0.2046301203171215</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.2096403935261369</v>
+        <v>0.1956943611878062</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.2199922817222123</v>
+        <v>0.2466881491246491</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.2204349446019456</v>
+        <v>0.2123710190639136</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.1652770648031216</v>
+        <v>0.1820696510099117</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.1863367111051463</v>
+        <v>0.210302979833812</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.1291021015699512</v>
+        <v>0.1794839063464464</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.2049447649760349</v>
+        <v>0.2233297240657419</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.2007773301522786</v>
+        <v>0.2393133728178417</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.2384123800495567</v>
+        <v>0.1629844592048781</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.2036775608132293</v>
+        <v>0.1969827144392482</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.2476979212442918</v>
+        <v>0.1965733061178754</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.2864219666562899</v>
+        <v>0.183836812759245</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.2442462490540736</v>
+        <v>0.1626435010973513</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.2091784137032771</v>
+        <v>0.1995352458803386</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.1845337331253921</v>
+        <v>0.2485047676408502</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.1927607344470286</v>
+        <v>0.2187800333905454</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.1696526789992195</v>
+        <v>0.2045486734926522</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.1614397292013895</v>
+        <v>0.1906019554497276</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.2130471213811032</v>
+        <v>0.2207784478459045</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.1846785523602854</v>
+        <v>0.2263140766664</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.1883170164149853</v>
+        <v>0.209776060412968</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.2499334586778545</v>
+        <v>0.2082701329743925</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.204048694661715</v>
+        <v>0.2040152875554088</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.1922779627043707</v>
+        <v>0.2138425143858722</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.149924146989616</v>
+        <v>0.1728289216916878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>